<commit_message>
Added new subject relationship HAD_INTERVENTION to data upload app and clinical parser.
</commit_message>
<xml_diff>
--- a/src/report_manager/apps/templates/ClinicalData_template.xlsx
+++ b/src/report_manager/apps/templates/ClinicalData_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plh450/Clinical_Proteomics/CKG/clinicalknowledgegraph/report_manager/apps/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plh450/Clinical_Proteomics/CKG/CKG/src/report_manager/apps/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C89E56B-D3AB-054C-989D-4A0C2E670B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBE9E01-6D71-0646-8D6A-27CC1410B7D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80240" yWindow="140" windowWidth="31140" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="31140" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>subject external_id</t>
   </si>
@@ -88,15 +88,9 @@
     <t>tissue</t>
   </si>
   <si>
-    <t>intervention</t>
-  </si>
-  <si>
     <t>disease</t>
   </si>
   <si>
-    <t>date of T2D diagnosis</t>
-  </si>
-  <si>
     <t>Biological sex (property) (qualifier value) (734000001)</t>
   </si>
   <si>
@@ -118,58 +112,22 @@
     <t>Diastole (90892000)</t>
   </si>
   <si>
-    <t>Waist circumference (276361009)</t>
-  </si>
-  <si>
     <t>Drug therapy (procedure) (416608005)</t>
   </si>
   <si>
-    <t>Lipid-lowering therapy (134350008)</t>
-  </si>
-  <si>
-    <t>NAFLD score</t>
-  </si>
-  <si>
-    <t>Fasting blood glucose level (271062006)</t>
-  </si>
-  <si>
-    <t>platelets/liter (277200003)</t>
-  </si>
-  <si>
-    <t>Bilirubin level (302787001)</t>
-  </si>
-  <si>
-    <t>Albumin measurement (26758005)</t>
-  </si>
-  <si>
-    <t>Alanine aminotransferase measurement (34608000)</t>
-  </si>
-  <si>
-    <t>Aspartate aminotransferase measurement (45896001)</t>
-  </si>
-  <si>
-    <t>Alkaline phosphatase measurement (88810008)</t>
-  </si>
-  <si>
-    <t>Gamma glutamyl transferase measurement (69480007)</t>
-  </si>
-  <si>
-    <t>Hemoglobin A1c measurement (43396009)</t>
-  </si>
-  <si>
-    <t>Total cholesterol:HDL ratio measurement (166842003)</t>
-  </si>
-  <si>
-    <t>High density lipoprotein measurement (17888004)</t>
-  </si>
-  <si>
-    <t>Low density lipoprotein cholesterol measurement (113079009)</t>
-  </si>
-  <si>
-    <t>VLDL cholesterol measurement (104585005)</t>
-  </si>
-  <si>
-    <t>Triglycerides measurement (14740000)</t>
+    <t>studies_intervention</t>
+  </si>
+  <si>
+    <t>had_intervention</t>
+  </si>
+  <si>
+    <t>had_intervention_type</t>
+  </si>
+  <si>
+    <t>had_intervention_in_combination</t>
+  </si>
+  <si>
+    <t>had_intervention_response</t>
   </si>
 </sst>
 </file>
@@ -553,67 +511,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX10"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="44" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="22" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="44" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="35" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="44" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="37" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="44" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,170 +564,136 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="2" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:50" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
-    <row r="10" spans="1:50" ht="16" x14ac:dyDescent="0.2">
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+    <row r="10" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>